<commit_message>
excel service, region slug removed
</commit_message>
<xml_diff>
--- a/dash-be/approved_regions.xlsx
+++ b/dash-be/approved_regions.xlsx
@@ -1,13 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ychopra/Desktop/dashboard-multi-acc/dash-be/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F322EB67-000B-6042-82A7-27FA17BF90BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="30220" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -58,14 +67,16 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="&quot;Nunito Sans&quot;"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>policy-cluster-6</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <rFont val="&quot;Nunito Sans&quot;"/>
       </rPr>
       <t>HA</t>
@@ -89,14 +100,16 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="&quot;Nunito Sans&quot;"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>jagruti-cluster-rc6-mar-21</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <rFont val="&quot;Nunito Sans&quot;"/>
       </rPr>
       <t>HA</t>
@@ -111,14 +124,16 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="&quot;Nunito Sans&quot;"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>3.1.0-rc7-latest</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <rFont val="&quot;Nunito Sans&quot;"/>
       </rPr>
       <t>HA</t>
@@ -127,14 +142,16 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="&quot;Nunito Sans&quot;"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>prod-small-groundcover</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <rFont val="&quot;Nunito Sans&quot;"/>
       </rPr>
       <t>HA</t>
@@ -149,14 +166,16 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="&quot;Nunito Sans&quot;"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>common-repo-cluster-mar25</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <rFont val="&quot;Nunito Sans&quot;"/>
       </rPr>
       <t>HA</t>
@@ -178,55 +197,73 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm"/>
   </numFmts>
-  <fonts count="9">
-    <font>
-      <sz val="10.0"/>
+  <fonts count="11">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="&quot;Nunito Sans&quot;"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="&quot;Nunito Sans&quot;"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="&quot;Nunito Sans&quot;"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF5BB3EA"/>
       <name val="&quot;Nunito Sans&quot;"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="&quot;Nunito Sans&quot;"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
+      <name val="&quot;Nunito Sans&quot;"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="&quot;Nunito Sans&quot;"/>
     </font>
   </fonts>
   <fills count="8">
@@ -234,7 +271,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -274,7 +311,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF515157"/>
@@ -285,70 +328,57 @@
       <top style="thin">
         <color rgb="FF515157"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -538,23 +568,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.38"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,349 +601,361 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1">
-        <v>-2.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="s">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="7">
-        <v>45717.24513888889</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="5">
+        <v>45717.245138888888</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="5">
         <v>45737.478472222225</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="7">
-        <v>45741.41388888889</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="C15" s="5">
+        <v>45741.413888888892</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="7">
-        <v>45741.57638888889</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="C16" s="5">
+        <v>45741.576388888891</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="7">
-        <v>45741.66805555556</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="C17" s="5">
+        <v>45741.668055555558</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="9"/>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A18" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A13"/>
-    <hyperlink r:id="rId2" ref="A14"/>
-    <hyperlink r:id="rId3" ref="A15"/>
-    <hyperlink r:id="rId4" ref="A16"/>
-    <hyperlink r:id="rId5" ref="A17"/>
+    <hyperlink ref="A13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A16" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A17" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
-  <drawing r:id="rId6"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A11:B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.88"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>31</v>
       </c>
     </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+    </row>
   </sheetData>
-  <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="B7:B10">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B1:B6">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="B1:B13" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>